<commit_message>
Bi-directional links; MW to GW and $ to M$; CO2 costs added to CCGT; Batteries costs updated; CO2 constraint updated.
</commit_message>
<xml_diff>
--- a/src/parameters/fuel_info.xlsx
+++ b/src/parameters/fuel_info.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\git_github\py_ggrid\src\tech_parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\git_github\py_ggrid\src\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="values" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -41,9 +41,6 @@
     <t>oil</t>
   </si>
   <si>
-    <t>€/MWhth</t>
-  </si>
-  <si>
     <t>CO2</t>
   </si>
   <si>
@@ -56,16 +53,29 @@
     <t>hard coal</t>
   </si>
   <si>
-    <t>t/MWh</t>
+    <t>kT/GWh</t>
+  </si>
+  <si>
+    <t>M€/GWhth</t>
+  </si>
+  <si>
+    <t>M€/kTCO2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -97,9 +107,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -399,15 +410,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -415,7 +426,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>35</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="C3">
         <v>0.22500000000000001</v>
@@ -426,7 +437,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2.5</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -434,10 +445,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="C5">
         <v>0.40300000000000002</v>
@@ -445,10 +456,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>8.5</v>
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="C6">
         <v>0.35399999999999998</v>
@@ -456,7 +467,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -470,7 +481,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>73</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="C8">
         <v>0.26400000000000001</v>
@@ -478,15 +489,23 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>45</v>
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B10" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Reindex CO2 budget fixed.
</commit_message>
<xml_diff>
--- a/src/parameters/fuel_info.xlsx
+++ b/src/parameters/fuel_info.xlsx
@@ -59,7 +59,7 @@
     <t>M€/GWhth</t>
   </si>
   <si>
-    <t>M€/kTCO2</t>
+    <t>M€/ktCO2</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -426,7 +426,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="C3">
         <v>0.22500000000000001</v>
@@ -492,7 +492,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="C9">
         <v>0</v>

</xml_diff>